<commit_message>
ADD CDD IDs To it
</commit_message>
<xml_diff>
--- a/Digital_Air_Conditional_Screen/Project Managment/Doc/RTM_Me.xlsx
+++ b/Digital_Air_Conditional_Screen/Project Managment/Doc/RTM_Me.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\embedded iti\software engineer\ddddd\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21960" windowHeight="8028"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Customer requirement ID</t>
   </si>
@@ -158,17 +154,41 @@
   </si>
   <si>
     <t>Hardware Requirment</t>
+  </si>
+  <si>
+    <t>CDD ID</t>
+  </si>
+  <si>
+    <t>EEPROM_01</t>
+  </si>
+  <si>
+    <t>EEPROM_02</t>
+  </si>
+  <si>
+    <t>TS_02</t>
+  </si>
+  <si>
+    <t>DIO_01</t>
+  </si>
+  <si>
+    <t>LCD_01</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>LCD_04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -177,7 +197,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -220,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -583,11 +603,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -646,18 +679,51 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -673,38 +739,23 @@
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -986,25 +1037,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.625" customWidth="1"/>
-    <col min="2" max="2" width="12.875" customWidth="1"/>
-    <col min="3" max="3" width="33.375" customWidth="1"/>
-    <col min="4" max="4" width="32.75" customWidth="1"/>
-    <col min="5" max="5" width="15.375" customWidth="1"/>
-    <col min="6" max="6" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="15.375" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" customWidth="1"/>
+    <col min="3" max="4" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1015,43 +1066,51 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+    <row r="2" spans="1:6" ht="9.75" customHeight="1">
+      <c r="A2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="32"/>
-    </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="32"/>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="D2" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="37"/>
+      <c r="F2" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="6" customHeight="1">
+      <c r="A3" s="28"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="43"/>
+    </row>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A4" s="28"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="43"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A5" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1060,58 +1119,68 @@
       <c r="C5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
-      <c r="B6" s="29" t="s">
+      <c r="D5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18" customHeight="1">
+      <c r="A6" s="30"/>
+      <c r="B6" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="28"/>
-    </row>
-    <row r="8" spans="1:5" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
-    </row>
-    <row r="9" spans="1:5" ht="7.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="10">
+      <c r="D6" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="44"/>
+      <c r="F6" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18" customHeight="1">
+      <c r="A7" s="30"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="39"/>
+    </row>
+    <row r="8" spans="1:6" ht="2.25" customHeight="1" thickBot="1">
+      <c r="A8" s="30"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="39"/>
+    </row>
+    <row r="9" spans="1:6" ht="7.5" hidden="1" customHeight="1">
+      <c r="A9" s="30"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="10.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="11">
+    <row r="10" spans="1:6" ht="10.5" hidden="1" customHeight="1">
+      <c r="A10" s="31"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="35" t="s">
+    <row r="11" spans="1:6" ht="0.75" customHeight="1">
+      <c r="A11" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -1120,116 +1189,141 @@
       <c r="C11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="9">
+      <c r="D11" s="25"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
+    <row r="12" spans="1:6">
+      <c r="A12" s="30"/>
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="36"/>
+      <c r="D12" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="30"/>
       <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="38"/>
+      <c r="D13" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="32"/>
       <c r="B14" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="38"/>
+      <c r="D14" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="32"/>
       <c r="B15" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="38"/>
+      <c r="D15" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="32"/>
       <c r="B16" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="38"/>
+      <c r="D16" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="32"/>
       <c r="B17" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="38"/>
+      <c r="D17" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="32"/>
       <c r="B18" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
+      <c r="D18" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A19" s="32"/>
       <c r="B19" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1">
       <c r="A20" s="16" t="s">
         <v>12</v>
       </c>
@@ -1239,12 +1333,15 @@
       <c r="C20" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" thickBot="1">
       <c r="A21" s="21" t="s">
         <v>35</v>
       </c>
@@ -1254,12 +1351,15 @@
       <c r="C21" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="23"/>
+      <c r="F21" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" thickBot="1">
       <c r="A22" s="21" t="s">
         <v>36</v>
       </c>
@@ -1269,12 +1369,15 @@
       <c r="C22" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="23"/>
+      <c r="F22" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" thickBot="1">
       <c r="A23" s="21" t="s">
         <v>37</v>
       </c>
@@ -1284,12 +1387,15 @@
       <c r="C23" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="23"/>
+      <c r="F23" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" thickBot="1">
       <c r="A24" s="21" t="s">
         <v>38</v>
       </c>
@@ -1299,31 +1405,37 @@
       <c r="C24" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D24" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="23"/>
+      <c r="F24" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="15" thickBot="1"/>
+    <row r="27" spans="1:6" ht="15" thickBot="1">
       <c r="B27" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D6:D7"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A11:A19"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="D6:D8"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Add Test Case Tags
</commit_message>
<xml_diff>
--- a/Digital_Air_Conditional_Screen/Project Managment/Doc/RTM_Me.xlsx
+++ b/Digital_Air_Conditional_Screen/Project Managment/Doc/RTM_Me.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21960" windowHeight="8028"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13284" windowHeight="6288"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
   <si>
     <t>Customer requirement ID</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Select_Modes</t>
   </si>
   <si>
-    <t>Decrease_Mode</t>
-  </si>
-  <si>
     <t xml:space="preserve">                                                              Out_Mode
 </t>
   </si>
@@ -178,6 +175,51 @@
   </si>
   <si>
     <t>LCD_04</t>
+  </si>
+  <si>
+    <t>TC_08</t>
+  </si>
+  <si>
+    <t>TC_09</t>
+  </si>
+  <si>
+    <t>TC_20</t>
+  </si>
+  <si>
+    <t>TC_21</t>
+  </si>
+  <si>
+    <t>TC_01,TC_02,TC_03,TC_04</t>
+  </si>
+  <si>
+    <t>TC_16</t>
+  </si>
+  <si>
+    <t>TC_18</t>
+  </si>
+  <si>
+    <t>TC_22</t>
+  </si>
+  <si>
+    <t>TC_10</t>
+  </si>
+  <si>
+    <t>Change_Mode</t>
+  </si>
+  <si>
+    <t>TC_26</t>
+  </si>
+  <si>
+    <t>TC_27</t>
+  </si>
+  <si>
+    <t>TC_05,TC_06</t>
+  </si>
+  <si>
+    <t>TC_28</t>
+  </si>
+  <si>
+    <t>TC_29</t>
   </si>
 </sst>
 </file>
@@ -202,18 +244,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -235,12 +271,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -583,17 +637,6 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -620,142 +663,171 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1039,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1059,370 +1131,407 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="9.75" customHeight="1">
+      <c r="A2" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="6" customHeight="1">
+      <c r="A3" s="47"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="38"/>
+    </row>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A4" s="47"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="38"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A5" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18" customHeight="1">
+      <c r="A6" s="49"/>
+      <c r="B6" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="9.75" customHeight="1">
-      <c r="A2" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="48" t="s">
+      <c r="E6" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18" customHeight="1">
+      <c r="A7" s="49"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="32"/>
+    </row>
+    <row r="8" spans="1:6" ht="2.25" customHeight="1" thickBot="1">
+      <c r="A8" s="49"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="32"/>
+    </row>
+    <row r="9" spans="1:6" ht="7.5" hidden="1" customHeight="1">
+      <c r="A9" s="49"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="10.5" hidden="1" customHeight="1">
+      <c r="A10" s="50"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="0.75" customHeight="1">
+      <c r="A11" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="49"/>
+      <c r="B12" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="49"/>
+      <c r="B13" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="42">
+      <c r="E13" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="6" customHeight="1">
-      <c r="A3" s="28"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="43"/>
-    </row>
-    <row r="4" spans="1:6" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A4" s="28"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="43"/>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A5" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="7" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="51"/>
+      <c r="B14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="51"/>
+      <c r="B15" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9">
+      <c r="E15" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" customHeight="1">
-      <c r="A6" s="30"/>
-      <c r="B6" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="39">
+    <row r="16" spans="1:6">
+      <c r="A16" s="51"/>
+      <c r="B16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" customHeight="1">
-      <c r="A7" s="30"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="39"/>
-    </row>
-    <row r="8" spans="1:6" ht="2.25" customHeight="1" thickBot="1">
-      <c r="A8" s="30"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="39"/>
-    </row>
-    <row r="9" spans="1:6" ht="7.5" hidden="1" customHeight="1">
-      <c r="A9" s="30"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="10.5" hidden="1" customHeight="1">
-      <c r="A10" s="31"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="0.75" customHeight="1">
-      <c r="A11" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="30"/>
-      <c r="B12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="10">
+    <row r="17" spans="1:6">
+      <c r="A17" s="51"/>
+      <c r="B17" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="30"/>
-      <c r="B13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="10">
+    <row r="18" spans="1:6">
+      <c r="A18" s="51"/>
+      <c r="B18" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="32"/>
-      <c r="B14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="24" t="s">
+    <row r="19" spans="1:6" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A19" s="51"/>
+      <c r="B19" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" thickBot="1">
+      <c r="A20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="10">
+      <c r="E20" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="32"/>
-      <c r="B15" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="10">
+    <row r="21" spans="1:6" ht="15" thickBot="1">
+      <c r="A21" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="32"/>
-      <c r="B16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="10">
+    <row r="22" spans="1:6" ht="15" thickBot="1">
+      <c r="A22" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="32"/>
-      <c r="B17" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="10">
+    <row r="23" spans="1:6" ht="15" thickBot="1">
+      <c r="A23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="32"/>
-      <c r="B18" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A19" s="32"/>
-      <c r="B19" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1">
-      <c r="A20" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="47" t="s">
+    <row r="24" spans="1:6" ht="15" thickBot="1">
+      <c r="A24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1">
-      <c r="A21" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="23"/>
-      <c r="F21" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1">
-      <c r="A22" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1">
-      <c r="A23" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="23"/>
-      <c r="F23" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1">
-      <c r="A24" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="23"/>
-      <c r="F24" s="18">
-        <v>1</v>
+      <c r="E24" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="9">
+        <v>0.75</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="15" thickBot="1"/>
     <row r="27" spans="1:6" ht="15" thickBot="1">
-      <c r="B27" s="6"/>
+      <c r="B27" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A11:A19"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="C6:C10"/>
@@ -1431,11 +1540,6 @@
     <mergeCell ref="E6:E8"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A11:A19"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>